<commit_message>
Correct L.Soulat's mistake on TTH4 libelle
</commit_message>
<xml_diff>
--- a/fonction_publique/assets/grilles_fonction_publique/corresp_neg_netneh_2018.xlsx
+++ b/fonction_publique/assets/grilles_fonction_publique/corresp_neg_netneh_2018.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ap.cdc.fr\RacineDFS\SERVICES\DDR\DSI\Fonction_Etudes\Carriere\Correspondance codes_CIR_neg\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11070"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="Sans lag" sheetId="2" r:id="rId1"/>
     <sheet name="Feuil1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2620" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2620" uniqueCount="423">
   <si>
     <t>code_grade_NEG</t>
   </si>
@@ -1291,12 +1286,15 @@
   </si>
   <si>
     <t>INFIRMIER EN SOINS GENER SPECIAL 4EME GR (CAT SEDENTAIRE)</t>
+  </si>
+  <si>
+    <t>adjoint technique principal de 1ère classe</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d/m/yyyy"/>
   </numFmts>
@@ -1655,7 +1653,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1665,7 +1663,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q19" sqref="Q19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2640,7 +2640,7 @@
         <v>102</v>
       </c>
       <c r="Q19" t="s">
-        <v>68</v>
+        <v>422</v>
       </c>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">

</xml_diff>